<commit_message>
Tanks: Forgot M prefix for M756 Tanks Model 33: Top level item now defined as M33M instead of drawing number Model 33: Remove self-reference in top level assembly
</commit_message>
<xml_diff>
--- a/OpsAndMats/Model33M.xlsx
+++ b/OpsAndMats/Model33M.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="237">
   <si>
     <t>Item</t>
   </si>
@@ -161,7 +161,7 @@
     <t>8029125-1</t>
   </si>
   <si>
-    <t>8027958</t>
+    <t>M33M</t>
   </si>
   <si>
     <t>WATER FILTER MTG. BRACKET MOD. 33</t>
@@ -1083,7 +1083,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AQ67"/>
+  <dimension ref="A1:AQ66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1901,10 +1901,10 @@
         <v>61</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1984,10 +1984,10 @@
         <v>61</v>
       </c>
       <c r="I11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K11">
         <v>2</v>
@@ -2067,7 +2067,7 @@
         <v>61</v>
       </c>
       <c r="I12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J12" t="s">
         <v>50</v>
@@ -2150,10 +2150,10 @@
         <v>61</v>
       </c>
       <c r="I13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K13">
         <v>4</v>
@@ -2233,10 +2233,10 @@
         <v>61</v>
       </c>
       <c r="I14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K14">
         <v>5</v>
@@ -2316,10 +2316,10 @@
         <v>61</v>
       </c>
       <c r="I15" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="J15" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="K15">
         <v>6</v>
@@ -2334,7 +2334,7 @@
         <v>8</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T15" t="s">
         <v>176</v>
@@ -2399,10 +2399,10 @@
         <v>61</v>
       </c>
       <c r="I16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K16">
         <v>7</v>
@@ -2417,7 +2417,7 @@
         <v>8</v>
       </c>
       <c r="S16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T16" t="s">
         <v>176</v>
@@ -2482,10 +2482,10 @@
         <v>61</v>
       </c>
       <c r="I17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J17" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K17">
         <v>8</v>
@@ -2500,7 +2500,7 @@
         <v>8</v>
       </c>
       <c r="S17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T17" t="s">
         <v>176</v>
@@ -2565,10 +2565,10 @@
         <v>61</v>
       </c>
       <c r="I18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J18" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K18">
         <v>9</v>
@@ -2583,7 +2583,7 @@
         <v>8</v>
       </c>
       <c r="S18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T18" t="s">
         <v>176</v>
@@ -2648,10 +2648,10 @@
         <v>61</v>
       </c>
       <c r="I19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K19">
         <v>10</v>
@@ -2731,10 +2731,10 @@
         <v>61</v>
       </c>
       <c r="I20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J20" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K20">
         <v>11</v>
@@ -2814,10 +2814,10 @@
         <v>61</v>
       </c>
       <c r="I21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J21" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K21">
         <v>12</v>
@@ -2897,10 +2897,10 @@
         <v>61</v>
       </c>
       <c r="I22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J22" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K22">
         <v>13</v>
@@ -2915,7 +2915,7 @@
         <v>8</v>
       </c>
       <c r="S22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T22" t="s">
         <v>176</v>
@@ -2980,10 +2980,10 @@
         <v>61</v>
       </c>
       <c r="I23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K23">
         <v>14</v>
@@ -2998,7 +2998,7 @@
         <v>8</v>
       </c>
       <c r="S23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T23" t="s">
         <v>176</v>
@@ -3063,10 +3063,10 @@
         <v>61</v>
       </c>
       <c r="I24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J24" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K24">
         <v>15</v>
@@ -3146,10 +3146,10 @@
         <v>61</v>
       </c>
       <c r="I25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J25" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="K25">
         <v>16</v>
@@ -3164,13 +3164,13 @@
         <v>8</v>
       </c>
       <c r="S25">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="T25" t="s">
         <v>176</v>
       </c>
       <c r="U25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="V25">
         <v>0</v>
@@ -3229,10 +3229,10 @@
         <v>61</v>
       </c>
       <c r="I26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K26">
         <v>17</v>
@@ -3312,10 +3312,10 @@
         <v>61</v>
       </c>
       <c r="I27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K27">
         <v>18</v>
@@ -3330,13 +3330,13 @@
         <v>8</v>
       </c>
       <c r="S27">
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="T27" t="s">
         <v>176</v>
       </c>
       <c r="U27" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="V27">
         <v>0</v>
@@ -3395,10 +3395,10 @@
         <v>61</v>
       </c>
       <c r="I28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J28" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K28">
         <v>19</v>
@@ -3478,10 +3478,10 @@
         <v>61</v>
       </c>
       <c r="I29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J29" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K29">
         <v>20</v>
@@ -3561,10 +3561,10 @@
         <v>61</v>
       </c>
       <c r="I30" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K30">
         <v>21</v>
@@ -3644,10 +3644,10 @@
         <v>61</v>
       </c>
       <c r="I31" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J31" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K31">
         <v>22</v>
@@ -3727,10 +3727,10 @@
         <v>61</v>
       </c>
       <c r="I32" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J32" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K32">
         <v>23</v>
@@ -3810,10 +3810,10 @@
         <v>61</v>
       </c>
       <c r="I33" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J33" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K33">
         <v>24</v>
@@ -3893,10 +3893,10 @@
         <v>61</v>
       </c>
       <c r="I34" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J34" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K34">
         <v>25</v>
@@ -3976,10 +3976,10 @@
         <v>61</v>
       </c>
       <c r="I35" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J35" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K35">
         <v>26</v>
@@ -4059,10 +4059,10 @@
         <v>61</v>
       </c>
       <c r="I36" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J36" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K36">
         <v>27</v>
@@ -4142,10 +4142,10 @@
         <v>61</v>
       </c>
       <c r="I37" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J37" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K37">
         <v>28</v>
@@ -4225,10 +4225,10 @@
         <v>61</v>
       </c>
       <c r="I38" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J38" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K38">
         <v>29</v>
@@ -4308,10 +4308,10 @@
         <v>61</v>
       </c>
       <c r="I39" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J39" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K39">
         <v>30</v>
@@ -4391,10 +4391,10 @@
         <v>61</v>
       </c>
       <c r="I40" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J40" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K40">
         <v>31</v>
@@ -4474,10 +4474,10 @@
         <v>61</v>
       </c>
       <c r="I41" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J41" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K41">
         <v>32</v>
@@ -4492,13 +4492,13 @@
         <v>8</v>
       </c>
       <c r="S41">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="T41" t="s">
         <v>176</v>
       </c>
       <c r="U41" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="V41">
         <v>0</v>
@@ -4557,10 +4557,10 @@
         <v>61</v>
       </c>
       <c r="I42" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J42" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K42">
         <v>33</v>
@@ -4575,13 +4575,13 @@
         <v>8</v>
       </c>
       <c r="S42">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="T42" t="s">
         <v>176</v>
       </c>
       <c r="U42" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="V42">
         <v>0</v>
@@ -4640,10 +4640,10 @@
         <v>61</v>
       </c>
       <c r="I43" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J43" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K43">
         <v>34</v>
@@ -4723,10 +4723,10 @@
         <v>61</v>
       </c>
       <c r="I44" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J44" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K44">
         <v>35</v>
@@ -4806,10 +4806,10 @@
         <v>61</v>
       </c>
       <c r="I45" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J45" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K45">
         <v>36</v>
@@ -4824,7 +4824,7 @@
         <v>8</v>
       </c>
       <c r="S45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T45" t="s">
         <v>176</v>
@@ -4889,10 +4889,10 @@
         <v>61</v>
       </c>
       <c r="I46" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J46" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K46">
         <v>37</v>
@@ -4907,7 +4907,7 @@
         <v>8</v>
       </c>
       <c r="S46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T46" t="s">
         <v>176</v>
@@ -4972,10 +4972,10 @@
         <v>61</v>
       </c>
       <c r="I47" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J47" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="K47">
         <v>38</v>
@@ -4990,7 +4990,7 @@
         <v>8</v>
       </c>
       <c r="S47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T47" t="s">
         <v>176</v>
@@ -5055,10 +5055,10 @@
         <v>61</v>
       </c>
       <c r="I48" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J48" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K48">
         <v>39</v>
@@ -5138,10 +5138,10 @@
         <v>61</v>
       </c>
       <c r="I49" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K49">
         <v>40</v>
@@ -5156,7 +5156,7 @@
         <v>8</v>
       </c>
       <c r="S49">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="T49" t="s">
         <v>176</v>
@@ -5221,10 +5221,10 @@
         <v>61</v>
       </c>
       <c r="I50" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J50" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="K50">
         <v>41</v>
@@ -5239,7 +5239,7 @@
         <v>8</v>
       </c>
       <c r="S50">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="T50" t="s">
         <v>176</v>
@@ -5304,10 +5304,10 @@
         <v>61</v>
       </c>
       <c r="I51" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J51" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K51">
         <v>42</v>
@@ -5322,7 +5322,7 @@
         <v>8</v>
       </c>
       <c r="S51">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="T51" t="s">
         <v>176</v>
@@ -5387,10 +5387,10 @@
         <v>61</v>
       </c>
       <c r="I52" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J52" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K52">
         <v>43</v>
@@ -5405,7 +5405,7 @@
         <v>8</v>
       </c>
       <c r="S52">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="T52" t="s">
         <v>176</v>
@@ -5470,10 +5470,10 @@
         <v>61</v>
       </c>
       <c r="I53" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J53" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K53">
         <v>44</v>
@@ -5553,10 +5553,10 @@
         <v>61</v>
       </c>
       <c r="I54" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J54" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K54">
         <v>45</v>
@@ -5571,7 +5571,7 @@
         <v>8</v>
       </c>
       <c r="S54">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="T54" t="s">
         <v>176</v>
@@ -5636,10 +5636,10 @@
         <v>61</v>
       </c>
       <c r="I55" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J55" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K55">
         <v>46</v>
@@ -5719,10 +5719,10 @@
         <v>61</v>
       </c>
       <c r="I56" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J56" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K56">
         <v>47</v>
@@ -5802,10 +5802,10 @@
         <v>61</v>
       </c>
       <c r="I57" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J57" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="K57">
         <v>48</v>
@@ -5885,10 +5885,10 @@
         <v>61</v>
       </c>
       <c r="I58" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J58" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="K58">
         <v>49</v>
@@ -5903,7 +5903,7 @@
         <v>8</v>
       </c>
       <c r="S58">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T58" t="s">
         <v>176</v>
@@ -5968,10 +5968,10 @@
         <v>61</v>
       </c>
       <c r="I59" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J59" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K59">
         <v>50</v>
@@ -5986,7 +5986,7 @@
         <v>8</v>
       </c>
       <c r="S59">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="T59" t="s">
         <v>176</v>
@@ -6051,10 +6051,10 @@
         <v>61</v>
       </c>
       <c r="I60" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J60" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K60">
         <v>51</v>
@@ -6069,7 +6069,7 @@
         <v>8</v>
       </c>
       <c r="S60">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="T60" t="s">
         <v>176</v>
@@ -6134,10 +6134,10 @@
         <v>61</v>
       </c>
       <c r="I61" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J61" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K61">
         <v>52</v>
@@ -6217,10 +6217,10 @@
         <v>61</v>
       </c>
       <c r="I62" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J62" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="K62">
         <v>53</v>
@@ -6300,10 +6300,10 @@
         <v>61</v>
       </c>
       <c r="I63" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J63" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K63">
         <v>54</v>
@@ -6383,10 +6383,10 @@
         <v>61</v>
       </c>
       <c r="I64" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J64" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K64">
         <v>55</v>
@@ -6466,10 +6466,10 @@
         <v>61</v>
       </c>
       <c r="I65" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J65" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="K65">
         <v>56</v>
@@ -6549,10 +6549,10 @@
         <v>61</v>
       </c>
       <c r="I66" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J66" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K66">
         <v>57</v>
@@ -6612,89 +6612,6 @@
         <v>0</v>
       </c>
       <c r="AQ66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:43">
-      <c r="A67" t="s">
-        <v>48</v>
-      </c>
-      <c r="B67" t="s">
-        <v>53</v>
-      </c>
-      <c r="E67">
-        <v>10</v>
-      </c>
-      <c r="G67" t="s">
-        <v>57</v>
-      </c>
-      <c r="H67" t="s">
-        <v>61</v>
-      </c>
-      <c r="I67" t="s">
-        <v>118</v>
-      </c>
-      <c r="J67" t="s">
-        <v>175</v>
-      </c>
-      <c r="K67">
-        <v>58</v>
-      </c>
-      <c r="L67">
-        <v>58</v>
-      </c>
-      <c r="M67">
-        <v>0</v>
-      </c>
-      <c r="R67" t="s">
-        <v>8</v>
-      </c>
-      <c r="S67">
-        <v>4</v>
-      </c>
-      <c r="T67" t="s">
-        <v>176</v>
-      </c>
-      <c r="U67" t="s">
-        <v>179</v>
-      </c>
-      <c r="V67">
-        <v>0</v>
-      </c>
-      <c r="W67">
-        <v>0</v>
-      </c>
-      <c r="AB67">
-        <v>1</v>
-      </c>
-      <c r="AF67">
-        <v>1</v>
-      </c>
-      <c r="AG67">
-        <v>0</v>
-      </c>
-      <c r="AH67">
-        <v>0</v>
-      </c>
-      <c r="AK67">
-        <v>0</v>
-      </c>
-      <c r="AL67">
-        <v>0</v>
-      </c>
-      <c r="AM67">
-        <v>0</v>
-      </c>
-      <c r="AN67">
-        <v>0</v>
-      </c>
-      <c r="AO67">
-        <v>0</v>
-      </c>
-      <c r="AP67">
-        <v>0</v>
-      </c>
-      <c r="AQ67">
         <v>0</v>
       </c>
     </row>

</xml_diff>